<commit_message>
check in SFDC using spritz
</commit_message>
<xml_diff>
--- a/PDFComparison/RunManager.xlsx
+++ b/PDFComparison/RunManager.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -62,12 +62,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>D:\Benchmark Report_ InvisiWrapper  AA_English_Mar.pdf</t>
-  </si>
-  <si>
-    <t>D:\Benchmark Report_ InvisiWrapper AA_English_Dec.pdf</t>
-  </si>
-  <si>
     <t>TestCase4</t>
   </si>
   <si>
@@ -83,7 +77,19 @@
     <t>D:\Options_10001933_Washington_4_2000Jun30.pdf</t>
   </si>
   <si>
-    <t>Test case 9</t>
+    <t>D:\Options_10001933_LUBY_3_2000Jun30_updated.pdf</t>
+  </si>
+  <si>
+    <t>D:\Options_10001933_LUBY_3_2000Jun30.pdf</t>
+  </si>
+  <si>
+    <t>TestCase6</t>
+  </si>
+  <si>
+    <t>D:\Benchmark 1–French.pdf</t>
+  </si>
+  <si>
+    <t>D:\Benchmark 1–French_New.pdf</t>
   </si>
 </sst>
 </file>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,72 +560,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated PDF compare codebase
</commit_message>
<xml_diff>
--- a/PDFComparison/RunManager.xlsx
+++ b/PDFComparison/RunManager.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Results (2)" sheetId="3" r:id="rId1"/>
     <sheet name="Results" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -99,6 +99,30 @@
   </si>
   <si>
     <t>D:\Test.pdf</t>
+  </si>
+  <si>
+    <t>TestCase7</t>
+  </si>
+  <si>
+    <t>D:\SIN_ADE.pdf</t>
+  </si>
+  <si>
+    <t>D:\SIN_UW.pdf</t>
+  </si>
+  <si>
+    <t>TestCase8</t>
+  </si>
+  <si>
+    <t>TestCase9</t>
+  </si>
+  <si>
+    <t>TestCase10</t>
+  </si>
+  <si>
+    <t>TestCase11</t>
+  </si>
+  <si>
+    <t>D:\ABRCIR-20180326.pdf</t>
   </si>
 </sst>
 </file>
@@ -539,10 +563,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,10 +596,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -592,7 +616,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -606,7 +630,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -620,7 +644,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -634,7 +658,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -648,7 +672,77 @@
         <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>